<commit_message>
Added more test scripts
</commit_message>
<xml_diff>
--- a/Config/TestData.xlsx
+++ b/Config/TestData.xlsx
@@ -1,41 +1,150 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sugandan\FionaAutomation\Config\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01658881-15EC-4BA6-91E2-51EF6ED07D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="39">
+  <si>
+    <t>PaymentDueBy</t>
+  </si>
+  <si>
+    <t>PaymentType</t>
+  </si>
+  <si>
+    <t>PaymentRegion</t>
+  </si>
+  <si>
+    <t>AccountType</t>
+  </si>
+  <si>
+    <t>AccountName</t>
+  </si>
+  <si>
+    <t>BeneficiaryName</t>
+  </si>
+  <si>
+    <t>SortCode</t>
+  </si>
+  <si>
+    <t>AccountNumber</t>
+  </si>
+  <si>
+    <t>IBAN</t>
+  </si>
+  <si>
+    <t>BIC</t>
+  </si>
+  <si>
+    <t>NetValue</t>
+  </si>
+  <si>
+    <t>VATApplicable</t>
+  </si>
+  <si>
+    <t>VATAmount</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Entity</t>
+  </si>
+  <si>
+    <t>NominalAccount</t>
+  </si>
+  <si>
+    <t>CostCentre</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>AdditionalComments_x000D_</t>
+  </si>
+  <si>
+    <t>10/12/2025</t>
+  </si>
+  <si>
+    <t>CHAPS (same day &gt; £250k)</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Office</t>
+  </si>
+  <si>
+    <t>Burlington Group Office - 14107168</t>
+  </si>
+  <si>
+    <t>11-15-55</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>IB123</t>
+  </si>
+  <si>
+    <t>BIC123</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>GBP - British Pound Sterling</t>
+  </si>
+  <si>
+    <t>MFSI</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>CC1</t>
+  </si>
+  <si>
+    <t>Test Desc</t>
+  </si>
+  <si>
+    <t>Optional comments_x000D_</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Jack Smith</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -65,13 +174,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,138 +513,312 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C3" sqref="A3:XFD3"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.09765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.8984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>PaymentDueBy</v>
-      </c>
-      <c r="B1" t="str">
-        <v>PaymentType</v>
-      </c>
-      <c r="C1" t="str">
-        <v>PaymentRegion</v>
-      </c>
-      <c r="D1" t="str">
-        <v>AccountType</v>
-      </c>
-      <c r="E1" t="str">
-        <v>AccountName</v>
-      </c>
-      <c r="F1" t="str">
-        <v>BeneficiaryName</v>
-      </c>
-      <c r="G1" t="str">
-        <v>SortCode</v>
-      </c>
-      <c r="H1" t="str">
-        <v>AccountNumber</v>
-      </c>
-      <c r="I1" t="str">
-        <v>IBAN</v>
-      </c>
-      <c r="J1" t="str">
-        <v>BIC</v>
-      </c>
-      <c r="K1" t="str">
-        <v>NetValue</v>
-      </c>
-      <c r="L1" t="str">
-        <v>VATApplicable</v>
-      </c>
-      <c r="M1" t="str">
-        <v>VATAmount</v>
-      </c>
-      <c r="N1" t="str">
-        <v>Currency</v>
-      </c>
-      <c r="O1" t="str">
-        <v>Entity</v>
-      </c>
-      <c r="P1" t="str">
-        <v>NominalAccount</v>
-      </c>
-      <c r="Q1" t="str">
-        <v>CostCentre</v>
-      </c>
-      <c r="R1" t="str">
-        <v>Description</v>
-      </c>
-      <c r="S1" t="str">
-        <v>AdditionalComments_x000d_</v>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>10/09/2025</v>
-      </c>
-      <c r="B2" t="str">
-        <v>CHAPS (same day &gt; £250k)</v>
-      </c>
-      <c r="C2" t="str">
-        <v>UK</v>
-      </c>
-      <c r="D2" t="str">
-        <v>Office</v>
-      </c>
-      <c r="E2" t="str">
-        <v>Burlington Group Office - 14107168</v>
-      </c>
-      <c r="F2" t="str">
-        <v>JohnDoe</v>
-      </c>
-      <c r="G2" t="str">
-        <v>11-15-55</v>
-      </c>
-      <c r="H2" t="str">
-        <v>12345678</v>
-      </c>
-      <c r="I2" t="str">
-        <v>IB123</v>
-      </c>
-      <c r="J2" t="str">
-        <v>BIC123</v>
-      </c>
-      <c r="K2" t="str">
-        <v>5000</v>
-      </c>
-      <c r="L2" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="M2" t="str">
-        <v>1000</v>
-      </c>
-      <c r="N2" t="str">
-        <v>GBP - British Pound Sterling</v>
-      </c>
-      <c r="O2" t="str">
-        <v>MFSI</v>
-      </c>
-      <c r="P2" t="str">
-        <v>12345</v>
-      </c>
-      <c r="Q2" t="str">
-        <v>CC1</v>
-      </c>
-      <c r="R2" t="str">
-        <v>Test Desc</v>
-      </c>
-      <c r="S2" t="str">
-        <v>Optional comments_x000d_</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v/>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:S3"/>
+    <ignoredError sqref="A1:S1 A2:E2 G2:S2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CE55B30-4C93-46AD-AAD5-EEBD68D7D6E9}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.09765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.8984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>